<commit_message>
criando a separacao de miscelaneas
</commit_message>
<xml_diff>
--- a/dados/regras/escala_de_atendimento_do_dia/escala_almoxarifado.xlsx
+++ b/dados/regras/escala_de_atendimento_do_dia/escala_almoxarifado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,240 +478,1080 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CLAUDIA PORTES BOHN</t>
+          <t>ALEXSANDRO SANTOS DE OLIVEIRA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z577892</t>
+          <t>Z563480</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>162352</v>
+        <v>161231</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>z577892</t>
+          <t>z563480</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EDSON BARROS DOS SANTOS</t>
+          <t>ANDERSON LUIS SOARES SARAIVA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Z562708</t>
+          <t>Z608155</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>160822</v>
+        <v>163206</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>FERNANDA GRAZIELE</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>z562708</t>
+          <t>z608155</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>FERNANDA GRAZIELE</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FABIO SILVA DOS SANTOS</t>
+          <t>CLAUDIA PORTES BOHN</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Z586158</t>
+          <t>Z577892</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>162400</v>
+        <v>162352</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>z586158</t>
+          <t>z577892</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JACQUES HELENO DE MATTOS</t>
+          <t>DAVID MANJOLI DE SOUZA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Z560055</t>
+          <t>Z563512</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>160829</v>
+        <v>161108</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>z560055</t>
+          <t>z563512</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NICOLAS GABRIEL TOGNI BENITES</t>
+          <t>DOUGLAS DE FREITAS FREITAS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Z562710</t>
+          <t>Z586156</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>160826</v>
+        <v>162401</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>FERNANDA GRAZIELE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>z562710</t>
+          <t>z586156</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>FERNANDA GRAZIELE</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>THOMAZ GABRIEL DE MELLO</t>
+          <t>FELIPE BANDEIRA DE FREITAS</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Z560066</t>
+          <t>Z600960</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>161030</v>
+        <v>162952</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GPON+HFC</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>QUA/SEX</t>
+          <t>SEG/ QUINTA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>z560066</t>
+          <t>z600960</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>JEFFERSON MELLO/ VT</t>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GREGORY ANDREY LIMA FERREIRA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Z560053</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>161059</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>z560053</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GUSTAVO SILVA DA SILVA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Z560054</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>161107</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>z560054</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>JORDAN DE FREITAS BATISTA SILVIERA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Z625774</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>162360</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>z625774</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JOSE THEODORO SILVA MARTINS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Z562061</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>160968</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>z562061</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LEANDRO STEFANI MOLINARI</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Z562709</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>160969</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>z562709</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LUCAS LACERDA OLIVEIRA</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Z571110</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>162151</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>z571110</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LUCKAN ROGER SCHIEFERDECKER NEVES</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Z563477</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>161433</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>z563477</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LUZIANE PENS GARCIA</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Z562071</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>160970</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>z562071</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MARCELO LEANDRO SILVA DA SILVA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Z583574</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>162272</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>z583574</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MARCUS VINICIUS COELHO LEITE</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Z583575</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>162361</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>z583575</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MATHEUS DE OLIVEIRA SEVERO</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Z560063</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>161230</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>z560063</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MATHEUS FRANCO COSTA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Z595262</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>162738</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>z595262</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MATHIAS BATISTA LIMA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Z563712</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>161470</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>z563712</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PATRICK GONÇALVES CANABARRO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Z625772</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>162931</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>z625772</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RAFAEL VARGAS SOUZA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Z608158</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>163205</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>z608158</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RENAN DA ROSA PEDROSO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Z600970</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>162922</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>z600970</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>VANDER CALISTRO OLIVEIRA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Z561915</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>161224</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>z561915</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>VINICIUS HONORATO DA CONCEICAO</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Z563468</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>161491</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>z563468</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WAGNER RICARDO SILVA TEIXEIRA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Z571113</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>162153</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>z571113</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WILLIAM MULLER DA LUZ</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Z601592</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>162946</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>z601592</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>JEFFERSON MELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>JAMILSON FREITAS COSTA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Z632498</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>163643</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>GPON+HFC</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>SEG/ QUINTA</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>z632498</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>FERNANDA GRAZIELE</t>
         </is>
       </c>
     </row>

</xml_diff>